<commit_message>
Jornada de usuario feito
</commit_message>
<xml_diff>
--- a/Documentação/Ata-Reunião/20220207_Reunião_Solluto.xlsx
+++ b/Documentação/Ata-Reunião/20220207_Reunião_Solluto.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoia\Desktop\Nova pasta\Sollute\Sollute\Ata-Reunião\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Júlia\Desktop\Sollute\Sollute\Documentação\Ata-Reunião\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C47C36A-B81F-4689-AC59-D1F02C63069A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -66,12 +65,6 @@
     <t>Gabriel Alves</t>
   </si>
   <si>
-    <t>Segunda-feira</t>
-  </si>
-  <si>
-    <t>Solute</t>
-  </si>
-  <si>
     <t>Guilherme Alemida</t>
   </si>
   <si>
@@ -84,13 +77,13 @@
     <t>Um progama desenvolvido para microempreendedores que precisam de uma solução em conta e que ajude com seus gerenciamentos</t>
   </si>
   <si>
-    <t>Decidimos o escopo do projeto. Discutimos sobre nosso cliente e nossos objetivos como produto</t>
-  </si>
-  <si>
-    <t>Ligar para empresa concorrentes e entender melhor como funciona a empresa</t>
-  </si>
-  <si>
     <t>Todos</t>
+  </si>
+  <si>
+    <t>Sollute</t>
+  </si>
+  <si>
+    <t>Terça-feira</t>
   </si>
   <si>
     <r>
@@ -148,11 +141,17 @@
       <t>: **</t>
     </r>
   </si>
+  <si>
+    <t>Decidimos o escopo do projeto. Discutimos sobre nosso cliente e nossos objetivos como produto</t>
+  </si>
+  <si>
+    <t>Ligar para empresa concorrentes e entender melhor como funciona a empresa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,7 +249,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,25 +270,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF605FAB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDB3EAF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFBEBDDD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2B8E1"/>
+        <fgColor rgb="FFDAD2F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3E00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,36 +488,36 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -557,10 +550,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,25 +613,25 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -649,16 +642,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3E00FF"/>
+      <color rgb="FFDAD2F1"/>
+      <color rgb="FF8F8EC4"/>
       <color rgb="FFF2B8E1"/>
       <color rgb="FFDB3EAF"/>
       <color rgb="FFBEBDDD"/>
-      <color rgb="FF8F8EC4"/>
       <color rgb="FF605FAB"/>
       <color rgb="FFDC164F"/>
       <color rgb="FF56A44F"/>
       <color rgb="FFFFE7F1"/>
-      <color rgb="FF421F49"/>
-      <color rgb="FFF6C6DC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -676,26 +669,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>588749</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>89646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>310042</xdr:colOff>
+      <xdr:colOff>281012</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Imagem 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -708,8 +695,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1379324" y="390525"/>
-          <a:ext cx="2769293" cy="1047750"/>
+          <a:off x="1568823" y="470646"/>
+          <a:ext cx="2522189" cy="862854"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1017,11 +1004,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:J17"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,20 +1018,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="13"/>
       <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1056,10 +1043,10 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
-      <c r="K2" s="5"/>
+      <c r="K2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -1069,10 +1056,10 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
-      <c r="K3" s="5"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -1082,10 +1069,10 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="5"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -1095,10 +1082,10 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="5"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -1108,10 +1095,10 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="5"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1121,10 +1108,10 @@
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1134,57 +1121,57 @@
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
-      <c r="K8" s="5"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="5"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="32" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
       <c r="J10" s="32"/>
-      <c r="K10" s="5"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="41" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="41"/>
       <c r="D11" s="41"/>
       <c r="E11" s="35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
       <c r="I11" s="35"/>
       <c r="J11" s="35"/>
-      <c r="K11" s="5"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
       <c r="D12" s="41"/>
@@ -1194,29 +1181,29 @@
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="34">
-        <v>44599</v>
+        <v>44615</v>
       </c>
       <c r="E13" s="34"/>
-      <c r="F13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="5"/>
+      <c r="F13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="32" t="s">
         <v>4</v>
       </c>
@@ -1228,10 +1215,10 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
-      <c r="K14" s="5"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="52" t="s">
         <v>12</v>
       </c>
@@ -1243,33 +1230,33 @@
       <c r="F15" s="38"/>
       <c r="G15" s="1"/>
       <c r="H15" s="38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I15" s="38"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="3"/>
       <c r="E16" s="39" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F16" s="39"/>
       <c r="G16" s="3"/>
       <c r="H16" s="40"/>
       <c r="I16" s="40"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="5"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
@@ -1279,23 +1266,23 @@
       <c r="H17" s="50"/>
       <c r="I17" s="50"/>
       <c r="J17" s="51"/>
-      <c r="K17" s="5"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="5"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
@@ -1307,26 +1294,26 @@
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="5"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="5"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
@@ -1334,12 +1321,12 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="5"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="26"/>
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
@@ -1347,12 +1334,12 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
       <c r="I22" s="28"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="5"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="26"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -1360,12 +1347,12 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
       <c r="I23" s="28"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="5"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="26"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
@@ -1373,12 +1360,12 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
       <c r="I24" s="28"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="5"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="26"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -1386,12 +1373,12 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
       <c r="I25" s="28"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="5"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="26"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
@@ -1399,12 +1386,12 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
       <c r="I26" s="28"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="5"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="26"/>
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
@@ -1412,12 +1399,12 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
       <c r="I27" s="28"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="5"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="26"/>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
@@ -1425,12 +1412,12 @@
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
       <c r="I28" s="28"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="5"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="29"/>
       <c r="D29" s="30"/>
       <c r="E29" s="30"/>
@@ -1438,24 +1425,24 @@
       <c r="G29" s="30"/>
       <c r="H29" s="30"/>
       <c r="I29" s="31"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="5"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="5"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="57" t="s">
         <v>8</v>
       </c>
@@ -1467,10 +1454,10 @@
       <c r="H31" s="57"/>
       <c r="I31" s="57"/>
       <c r="J31" s="57"/>
-      <c r="K31" s="5"/>
+      <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="58" t="s">
         <v>7</v>
       </c>
@@ -1486,29 +1473,29 @@
         <v>10</v>
       </c>
       <c r="J32" s="60"/>
-      <c r="K32" s="5"/>
+      <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="48" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
       <c r="F33" s="48"/>
       <c r="G33" s="46" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H33" s="46"/>
       <c r="I33" s="42">
         <v>44610</v>
       </c>
       <c r="J33" s="42"/>
-      <c r="K33" s="5"/>
+      <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
@@ -1518,10 +1505,10 @@
       <c r="H34" s="46"/>
       <c r="I34" s="42"/>
       <c r="J34" s="42"/>
-      <c r="K34" s="5"/>
+      <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
       <c r="D35" s="48"/>
@@ -1531,10 +1518,10 @@
       <c r="H35" s="46"/>
       <c r="I35" s="42"/>
       <c r="J35" s="42"/>
-      <c r="K35" s="5"/>
+      <c r="K35" s="14"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="13"/>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
       <c r="D36" s="48"/>
@@ -1544,10 +1531,10 @@
       <c r="H36" s="46"/>
       <c r="I36" s="42"/>
       <c r="J36" s="42"/>
-      <c r="K36" s="5"/>
+      <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
       <c r="D37" s="48"/>
@@ -1557,10 +1544,10 @@
       <c r="H37" s="46"/>
       <c r="I37" s="42"/>
       <c r="J37" s="42"/>
-      <c r="K37" s="5"/>
+      <c r="K37" s="14"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
       <c r="D38" s="48"/>
@@ -1570,10 +1557,10 @@
       <c r="H38" s="46"/>
       <c r="I38" s="42"/>
       <c r="J38" s="42"/>
-      <c r="K38" s="5"/>
+      <c r="K38" s="14"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="47"/>
       <c r="C39" s="47"/>
       <c r="D39" s="47"/>
@@ -1583,10 +1570,10 @@
       <c r="H39" s="44"/>
       <c r="I39" s="45"/>
       <c r="J39" s="45"/>
-      <c r="K39" s="5"/>
+      <c r="K39" s="14"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="47"/>
       <c r="C40" s="47"/>
       <c r="D40" s="47"/>
@@ -1596,10 +1583,10 @@
       <c r="H40" s="44"/>
       <c r="I40" s="45"/>
       <c r="J40" s="45"/>
-      <c r="K40" s="5"/>
+      <c r="K40" s="14"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="47"/>
       <c r="C41" s="47"/>
       <c r="D41" s="47"/>
@@ -1609,10 +1596,10 @@
       <c r="H41" s="44"/>
       <c r="I41" s="45"/>
       <c r="J41" s="45"/>
-      <c r="K41" s="5"/>
+      <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="47"/>
       <c r="C42" s="47"/>
       <c r="D42" s="47"/>
@@ -1622,10 +1609,10 @@
       <c r="H42" s="44"/>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
-      <c r="K42" s="5"/>
+      <c r="K42" s="14"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="47"/>
       <c r="C43" s="47"/>
       <c r="D43" s="47"/>
@@ -1635,10 +1622,10 @@
       <c r="H43" s="44"/>
       <c r="I43" s="45"/>
       <c r="J43" s="45"/>
-      <c r="K43" s="5"/>
+      <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="47"/>
       <c r="C44" s="47"/>
       <c r="D44" s="47"/>
@@ -1648,10 +1635,10 @@
       <c r="H44" s="44"/>
       <c r="I44" s="45"/>
       <c r="J44" s="45"/>
-      <c r="K44" s="5"/>
+      <c r="K44" s="14"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="43"/>
       <c r="C45" s="43"/>
       <c r="D45" s="43"/>
@@ -1661,10 +1648,10 @@
       <c r="H45" s="44"/>
       <c r="I45" s="45"/>
       <c r="J45" s="45"/>
-      <c r="K45" s="5"/>
+      <c r="K45" s="14"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
       <c r="D46" s="43"/>
@@ -1674,10 +1661,10 @@
       <c r="H46" s="44"/>
       <c r="I46" s="45"/>
       <c r="J46" s="45"/>
-      <c r="K46" s="5"/>
+      <c r="K46" s="14"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
       <c r="D47" s="43"/>
@@ -1687,10 +1674,10 @@
       <c r="H47" s="44"/>
       <c r="I47" s="45"/>
       <c r="J47" s="45"/>
-      <c r="K47" s="5"/>
+      <c r="K47" s="14"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="55" t="s">
         <v>11</v>
       </c>
@@ -1699,15 +1686,15 @@
         <v>44610</v>
       </c>
       <c r="E48" s="55"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="5"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="14"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="54"/>
       <c r="C49" s="54"/>
       <c r="D49" s="54"/>
@@ -1716,21 +1703,21 @@
       <c r="G49" s="54"/>
       <c r="H49" s="54"/>
       <c r="I49" s="54"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="5"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="14"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="11"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="43">

</xml_diff>